<commit_message>
Fix duplicate PersistenceUtils error: Removed stray PersistenceUtils class from Enquiry.java and corrected file structure corrected file reading and struture
</commit_message>
<xml_diff>
--- a/test/ApplicantsList.xlsx
+++ b/test/ApplicantsList.xlsx
@@ -113,12 +113,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="4.44140625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="13.59375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="12.96875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.62890625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.62890625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="4.58984375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.7890625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.28125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="13.12890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Fixed the no projects found problem
</commit_message>
<xml_diff>
--- a/test/ApplicantsList.xlsx
+++ b/test/ApplicantsList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -32,37 +32,82 @@
     <t>User Type</t>
   </si>
   <si>
+    <t>John</t>
+  </si>
+  <si>
     <t>S1234567A</t>
   </si>
   <si>
-    <t>SINGLE</t>
-  </si>
-  <si>
-    <t>password123</t>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
   <si>
     <t>Applicant</t>
   </si>
   <si>
-    <t>S9876543B</t>
-  </si>
-  <si>
-    <t>MARRIED</t>
-  </si>
-  <si>
-    <t>manager123</t>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>T7654321B</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>S9876543C</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>T2345678D</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>S3456789E</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>T8765432F</t>
   </si>
   <si>
     <t>HDBManager</t>
   </si>
   <si>
-    <t>S5555555F</t>
-  </si>
-  <si>
-    <t>officer123</t>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>S5678901G</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>T2109876H</t>
   </si>
   <si>
     <t>HDBOfficer</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>S6543210I</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>T1234567J</t>
   </si>
 </sst>
 </file>
@@ -107,17 +152,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.62890625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.62890625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="8.06640625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.79296875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="4.58984375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.7890625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="13.28125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="9.78125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="13.12890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -146,39 +191,39 @@
         <v>6</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>30.0</v>
+        <v>35.0</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>45.0</v>
+        <v>40.0</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -186,19 +231,159 @@
         <v>14</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>40.0</v>
+        <v>37.0</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>16</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>25.0</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>36.0</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>36.0</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>28.0</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>